<commit_message>
chore: add information from Nekraus for the motor messages
</commit_message>
<xml_diff>
--- a/chip_list.xlsx
+++ b/chip_list.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t xml:space="preserve">UC ID</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>https://www.winbond.com/resource-files/W25Q32JV%20RevI%2005042021%20Plus.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERIAL FLASH MEMORY</t>
   </si>
   <si>
     <t>U12</t>
@@ -227,7 +230,6 @@
     </font>
     <font>
       <sz val="10.000000"/>
-      <color indexed="64"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -273,7 +275,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="2" borderId="1" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -286,17 +288,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -949,43 +949,46 @@
       <c r="D12" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="E12" s="6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="13" ht="28.5">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" ht="28.5">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" ht="28.5">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -994,104 +997,104 @@
     </row>
     <row r="16" ht="28.5">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" ht="14.25"/>
     <row r="19" ht="28.5">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="7" t="s">
+      <c r="A20" s="5" t="s">
         <v>52</v>
       </c>
+      <c r="B20" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="C20" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" ht="28.5">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" ht="14.25">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="9" t="s">
         <v>53</v>
       </c>
+      <c r="C22" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="D22" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" ht="14.25">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="A27" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" t="s">
         <v>59</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="C27" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="27" ht="14.25">
-      <c r="A27" s="10" t="s">
+      <c r="D27" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="B27" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="28" ht="14.25"/>

</xml_diff>